<commit_message>
think i have fixed all bugs, added two non-implemented DERS functions without peak consideration
</commit_message>
<xml_diff>
--- a/MonteCarloResultsBUS6Sub2M.xlsx
+++ b/MonteCarloResultsBUS6Sub2M.xlsx
@@ -145,10 +145,10 @@
     <t>farm</t>
   </si>
   <si>
-    <t>(49.357797109377685, 53.57182189112085)</t>
-  </si>
-  <si>
-    <t>(48.69559321510376, 54.23402578539477)</t>
+    <t>(51.07192742410905, 55.28471085596654)</t>
+  </si>
+  <si>
+    <t>(50.40991859910287, 55.94671968097271)</t>
   </si>
 </sst>
 </file>
@@ -582,28 +582,28 @@
         <v>147</v>
       </c>
       <c r="F2">
-        <v>7.178425322073187</v>
+        <v>7.572506307224296</v>
       </c>
       <c r="G2">
-        <v>3466</v>
+        <v>3415</v>
       </c>
       <c r="H2">
-        <v>5.426276498508872</v>
+        <v>5.765304948399171</v>
       </c>
       <c r="I2">
-        <v>1.322900763358779</v>
+        <v>1.313461538461538</v>
       </c>
       <c r="J2">
-        <v>194.4664122137405</v>
+        <v>193.0788461538461</v>
       </c>
       <c r="K2">
-        <v>1055.228522344758</v>
+        <v>1113.158427161972</v>
       </c>
       <c r="L2">
-        <v>797.6626452808042</v>
+        <v>847.4998274146782</v>
       </c>
       <c r="M2">
-        <v>1.190900760931942</v>
+        <v>1.25627879636851</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -623,28 +623,28 @@
         <v>126</v>
       </c>
       <c r="F3">
-        <v>7.033498664578222</v>
+        <v>7.55268244677915</v>
       </c>
       <c r="G3">
-        <v>3447</v>
+        <v>3409</v>
       </c>
       <c r="H3">
-        <v>5.346030316563661</v>
+        <v>5.760332754950364</v>
       </c>
       <c r="I3">
-        <v>1.315648854961832</v>
+        <v>1.311153846153846</v>
       </c>
       <c r="J3">
-        <v>165.7717557251908</v>
+        <v>165.2053846153846</v>
       </c>
       <c r="K3">
-        <v>886.220831736856</v>
+        <v>951.6379882941729</v>
       </c>
       <c r="L3">
-        <v>673.5998198870213</v>
+        <v>725.8019271237459</v>
       </c>
       <c r="M3">
-        <v>1.271656558555742</v>
+        <v>1.36552498637767</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -664,28 +664,28 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>7.124772527760832</v>
+        <v>7.50043214450328</v>
       </c>
       <c r="G4">
-        <v>3450</v>
+        <v>3414</v>
       </c>
       <c r="H4">
-        <v>5.410696818183588</v>
+        <v>5.712104152228625</v>
       </c>
       <c r="I4">
-        <v>1.316793893129771</v>
+        <v>1.313076923076923</v>
       </c>
       <c r="J4">
-        <v>1.316793893129771</v>
+        <v>1.313076923076923</v>
       </c>
       <c r="K4">
-        <v>7.124772527760832</v>
+        <v>7.50043214450328</v>
       </c>
       <c r="L4">
-        <v>5.410696818183588</v>
+        <v>5.712104152228625</v>
       </c>
       <c r="M4">
-        <v>1.781905609192984</v>
+        <v>1.87585807934027</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -705,28 +705,28 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>7.105124786399911</v>
+        <v>7.534238085261641</v>
       </c>
       <c r="G5">
-        <v>3452</v>
+        <v>3414</v>
       </c>
       <c r="H5">
-        <v>5.392649750975599</v>
+        <v>5.737849742730013</v>
       </c>
       <c r="I5">
-        <v>1.317557251908397</v>
+        <v>1.313076923076923</v>
       </c>
       <c r="J5">
-        <v>1.317557251908397</v>
+        <v>1.313076923076923</v>
       </c>
       <c r="K5">
-        <v>7.105124786399911</v>
+        <v>7.534238085261641</v>
       </c>
       <c r="L5">
-        <v>5.392649750975599</v>
+        <v>5.737849742730013</v>
       </c>
       <c r="M5">
-        <v>1.870779356259096</v>
+        <v>1.98376488784939</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -746,28 +746,28 @@
         <v>132</v>
       </c>
       <c r="F6">
-        <v>8.357090670560375</v>
+        <v>8.878141583495536</v>
       </c>
       <c r="G6">
-        <v>3446</v>
+        <v>3417</v>
       </c>
       <c r="H6">
-        <v>6.35391107279982</v>
+        <v>6.755390142548549</v>
       </c>
       <c r="I6">
-        <v>1.315267175572519</v>
+        <v>1.314230769230769</v>
       </c>
       <c r="J6">
-        <v>173.6152671755725</v>
+        <v>173.4784615384615</v>
       </c>
       <c r="K6">
-        <v>1103.135968513969</v>
+        <v>1171.914689021411</v>
       </c>
       <c r="L6">
-        <v>838.7162616095763</v>
+        <v>891.7114988164085</v>
       </c>
       <c r="M6">
-        <v>1.729917768805997</v>
+        <v>1.837775307783576</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -787,28 +787,28 @@
         <v>147</v>
       </c>
       <c r="F7">
-        <v>8.777599545237562</v>
+        <v>9.024545432902086</v>
       </c>
       <c r="G7">
-        <v>3537</v>
+        <v>3482</v>
       </c>
       <c r="H7">
-        <v>6.501925589064861</v>
+        <v>6.738603712103798</v>
       </c>
       <c r="I7">
-        <v>1.35</v>
+        <v>1.339230769230769</v>
       </c>
       <c r="J7">
-        <v>198.45</v>
+        <v>196.8669230769231</v>
       </c>
       <c r="K7">
-        <v>1290.307133149922</v>
+        <v>1326.608178636607</v>
       </c>
       <c r="L7">
-        <v>955.7830615925345</v>
+        <v>990.5747456792583</v>
       </c>
       <c r="M7">
-        <v>1.456203764554912</v>
+        <v>1.497172087318456</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -828,28 +828,28 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>8.644351441768917</v>
+        <v>9.006205375083971</v>
       </c>
       <c r="G8">
-        <v>3540</v>
+        <v>3482</v>
       </c>
       <c r="H8">
-        <v>6.397796829783775</v>
+        <v>6.724909240441793</v>
       </c>
       <c r="I8">
-        <v>1.351145038167939</v>
+        <v>1.339230769230769</v>
       </c>
       <c r="J8">
-        <v>1.351145038167939</v>
+        <v>1.339230769230769</v>
       </c>
       <c r="K8">
-        <v>8.644351441768917</v>
+        <v>9.006205375083971</v>
       </c>
       <c r="L8">
-        <v>6.397796829783775</v>
+        <v>6.724909240441793</v>
       </c>
       <c r="M8">
-        <v>2.642578235748758</v>
+        <v>2.75319698316317</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -869,28 +869,28 @@
         <v>79</v>
       </c>
       <c r="F9">
-        <v>8.476161673255783</v>
+        <v>8.850115772952966</v>
       </c>
       <c r="G9">
-        <v>3459</v>
+        <v>3409</v>
       </c>
       <c r="H9">
-        <v>6.42022075279854</v>
+        <v>6.749868292659934</v>
       </c>
       <c r="I9">
-        <v>1.320229007633588</v>
+        <v>1.311153846153846</v>
       </c>
       <c r="J9">
-        <v>104.2980916030534</v>
+        <v>103.5811538461538</v>
       </c>
       <c r="K9">
-        <v>669.6167721872068</v>
+        <v>699.1591460632843</v>
       </c>
       <c r="L9">
-        <v>507.1974394710847</v>
+        <v>533.2395951201348</v>
       </c>
       <c r="M9">
-        <v>1.317195524023949</v>
+        <v>1.375307991116891</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -910,28 +910,28 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>10.76589156413828</v>
+        <v>11.16145205226164</v>
       </c>
       <c r="G10">
-        <v>3525</v>
+        <v>3491</v>
       </c>
       <c r="H10">
-        <v>8.001882524267319</v>
+        <v>8.312739998819898</v>
       </c>
       <c r="I10">
-        <v>1.345419847328244</v>
+        <v>1.342692307692308</v>
       </c>
       <c r="J10">
-        <v>1.345419847328244</v>
+        <v>1.342692307692308</v>
       </c>
       <c r="K10">
-        <v>10.76589156413828</v>
+        <v>11.16145205226164</v>
       </c>
       <c r="L10">
-        <v>8.001882524267319</v>
+        <v>8.312739998819898</v>
       </c>
       <c r="M10">
-        <v>3.047823901807548</v>
+        <v>3.159807075995271</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -951,28 +951,28 @@
         <v>76</v>
       </c>
       <c r="F11">
-        <v>10.66749364915747</v>
+        <v>10.89486911554118</v>
       </c>
       <c r="G11">
-        <v>3462</v>
+        <v>3413</v>
       </c>
       <c r="H11">
-        <v>8.073031011205247</v>
+        <v>8.299636595489909</v>
       </c>
       <c r="I11">
-        <v>1.321374045801527</v>
+        <v>1.312692307692308</v>
       </c>
       <c r="J11">
-        <v>100.424427480916</v>
+        <v>99.76461538461538</v>
       </c>
       <c r="K11">
-        <v>810.7295173359676</v>
+        <v>828.0100527811294</v>
       </c>
       <c r="L11">
-        <v>613.5503568515987</v>
+        <v>630.7723812572331</v>
       </c>
       <c r="M11">
-        <v>1.690797743391459</v>
+        <v>1.726836754813277</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -992,28 +992,28 @@
         <v>79</v>
       </c>
       <c r="F12">
-        <v>11.7968079213973</v>
+        <v>12.21462677222745</v>
       </c>
       <c r="G12">
-        <v>3830</v>
+        <v>3812</v>
       </c>
       <c r="H12">
-        <v>8.069879048057686</v>
+        <v>8.331067578119454</v>
       </c>
       <c r="I12">
-        <v>1.461832061068702</v>
+        <v>1.466153846153846</v>
       </c>
       <c r="J12">
-        <v>115.4847328244275</v>
+        <v>115.8261538461538</v>
       </c>
       <c r="K12">
-        <v>931.947825790387</v>
+        <v>964.9555150059682</v>
       </c>
       <c r="L12">
-        <v>637.5204447965572</v>
+        <v>658.1543386714368</v>
       </c>
       <c r="M12">
-        <v>1.833223950985141</v>
+        <v>1.898153000404145</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1033,28 +1033,28 @@
         <v>76</v>
       </c>
       <c r="F13">
-        <v>11.78143867646495</v>
+        <v>12.21315217615776</v>
       </c>
       <c r="G13">
-        <v>3830</v>
+        <v>3817</v>
       </c>
       <c r="H13">
-        <v>8.059365360923804</v>
+        <v>8.319150028297139</v>
       </c>
       <c r="I13">
-        <v>1.461832061068702</v>
+        <v>1.468076923076923</v>
       </c>
       <c r="J13">
-        <v>111.0992366412214</v>
+        <v>111.5738461538461</v>
       </c>
       <c r="K13">
-        <v>895.3893394113363</v>
+        <v>928.1995653879899</v>
       </c>
       <c r="L13">
-        <v>612.5117674302091</v>
+        <v>632.2554021505825</v>
       </c>
       <c r="M13">
-        <v>1.867358030219695</v>
+        <v>1.935784619921005</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1074,28 +1074,28 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>12.82656010509266</v>
+        <v>13.08832600787552</v>
       </c>
       <c r="G14">
-        <v>4154</v>
+        <v>4122</v>
       </c>
       <c r="H14">
-        <v>8.089934394641972</v>
+        <v>8.255615628451324</v>
       </c>
       <c r="I14">
-        <v>1.585496183206107</v>
+        <v>1.585384615384615</v>
       </c>
       <c r="J14">
-        <v>1.585496183206107</v>
+        <v>1.585384615384615</v>
       </c>
       <c r="K14">
-        <v>12.82656010509266</v>
+        <v>13.08832600787552</v>
       </c>
       <c r="L14">
-        <v>8.089934394641972</v>
+        <v>8.255615628451324</v>
       </c>
       <c r="M14">
-        <v>3.207922682283673</v>
+        <v>3.273390334569668</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1115,28 +1115,28 @@
         <v>79</v>
       </c>
       <c r="F15">
-        <v>11.07652364103258</v>
+        <v>11.44023702710331</v>
       </c>
       <c r="G15">
-        <v>4230</v>
+        <v>4268</v>
       </c>
       <c r="H15">
-        <v>6.86063639231805</v>
+        <v>6.969216558216638</v>
       </c>
       <c r="I15">
-        <v>1.614503816793893</v>
+        <v>1.641538461538462</v>
       </c>
       <c r="J15">
-        <v>127.5458015267176</v>
+        <v>129.6815384615385</v>
       </c>
       <c r="K15">
-        <v>875.0453676415736</v>
+        <v>903.7787251411615</v>
       </c>
       <c r="L15">
-        <v>541.990274993126</v>
+        <v>550.5681080991144</v>
       </c>
       <c r="M15">
-        <v>1.721291773816463</v>
+        <v>1.777812834011855</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1156,28 +1156,28 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>11.25232783887177</v>
+        <v>11.54427496778571</v>
       </c>
       <c r="G16">
-        <v>4310</v>
+        <v>4329</v>
       </c>
       <c r="H16">
-        <v>6.840162166553144</v>
+        <v>6.933498479150579</v>
       </c>
       <c r="I16">
-        <v>1.645038167938931</v>
+        <v>1.665</v>
       </c>
       <c r="J16">
-        <v>1.645038167938931</v>
+        <v>1.665</v>
       </c>
       <c r="K16">
-        <v>11.25232783887177</v>
+        <v>11.54427496778571</v>
       </c>
       <c r="L16">
-        <v>6.840162166553144</v>
+        <v>6.933498479150579</v>
       </c>
       <c r="M16">
-        <v>2.170574040118365</v>
+        <v>2.226890641285864</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1197,28 +1197,28 @@
         <v>76</v>
       </c>
       <c r="F17">
-        <v>11.08732390344275</v>
+        <v>11.41800602768974</v>
       </c>
       <c r="G17">
-        <v>4224</v>
+        <v>4267</v>
       </c>
       <c r="H17">
-        <v>6.877080640866479</v>
+        <v>6.957303883757518</v>
       </c>
       <c r="I17">
-        <v>1.612213740458015</v>
+        <v>1.641153846153846</v>
       </c>
       <c r="J17">
-        <v>122.5282442748092</v>
+        <v>124.7276923076923</v>
       </c>
       <c r="K17">
-        <v>842.6366166616491</v>
+        <v>867.7684581044205</v>
       </c>
       <c r="L17">
-        <v>522.6581287058524</v>
+        <v>528.7550951655714</v>
       </c>
       <c r="M17">
-        <v>1.757340838695676</v>
+        <v>1.809753955388824</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1238,28 +1238,28 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>10.98611871425499</v>
+        <v>11.38806946575303</v>
       </c>
       <c r="G18">
-        <v>4220</v>
+        <v>4260</v>
       </c>
       <c r="H18">
-        <v>6.820765647238883</v>
+        <v>6.950464932149737</v>
       </c>
       <c r="I18">
-        <v>1.610687022900763</v>
+        <v>1.638461538461538</v>
       </c>
       <c r="J18">
-        <v>1.610687022900763</v>
+        <v>1.638461538461538</v>
       </c>
       <c r="K18">
-        <v>10.98611871425499</v>
+        <v>11.38806946575303</v>
       </c>
       <c r="L18">
-        <v>6.820765647238883</v>
+        <v>6.950464932149737</v>
       </c>
       <c r="M18">
-        <v>2.747628290435174</v>
+        <v>2.848156173384833</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -1279,28 +1279,28 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>12.04595184124583</v>
+        <v>12.60236766102066</v>
       </c>
       <c r="G19">
-        <v>4580</v>
+        <v>4641</v>
       </c>
       <c r="H19">
-        <v>6.890915682110058</v>
+        <v>7.060149950151633</v>
       </c>
       <c r="I19">
-        <v>1.748091603053435</v>
+        <v>1.785</v>
       </c>
       <c r="J19">
-        <v>1.748091603053435</v>
+        <v>1.785</v>
       </c>
       <c r="K19">
-        <v>12.04595184124583</v>
+        <v>12.60236766102066</v>
       </c>
       <c r="L19">
-        <v>6.890915682110058</v>
+        <v>7.060149950151633</v>
       </c>
       <c r="M19">
-        <v>3.171699119800026</v>
+        <v>3.318203405146741</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -1320,28 +1320,28 @@
         <v>79</v>
       </c>
       <c r="F20">
-        <v>13.40512771731994</v>
+        <v>13.61299186526415</v>
       </c>
       <c r="G20">
-        <v>4322</v>
+        <v>4242</v>
       </c>
       <c r="H20">
-        <v>8.126199588009774</v>
+        <v>8.34365366564988</v>
       </c>
       <c r="I20">
-        <v>1.649618320610687</v>
+        <v>1.631538461538462</v>
       </c>
       <c r="J20">
-        <v>130.3198473282443</v>
+        <v>128.8915384615385</v>
       </c>
       <c r="K20">
-        <v>1059.005089668275</v>
+        <v>1075.426357355868</v>
       </c>
       <c r="L20">
-        <v>641.9697674527721</v>
+        <v>659.1486395863406</v>
       </c>
       <c r="M20">
-        <v>2.083156847271519</v>
+        <v>2.115458935862049</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -1361,28 +1361,28 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>13.52323654352755</v>
+        <v>13.74589299891787</v>
       </c>
       <c r="G21">
-        <v>4412</v>
+        <v>4319</v>
       </c>
       <c r="H21">
-        <v>8.030571111523615</v>
+        <v>8.274906644405293</v>
       </c>
       <c r="I21">
-        <v>1.683969465648855</v>
+        <v>1.661153846153846</v>
       </c>
       <c r="J21">
-        <v>1.683969465648855</v>
+        <v>1.661153846153846</v>
       </c>
       <c r="K21">
-        <v>13.52323654352755</v>
+        <v>13.74589299891787</v>
       </c>
       <c r="L21">
-        <v>8.030571111523615</v>
+        <v>8.274906644405293</v>
       </c>
       <c r="M21">
-        <v>2.608632329246465</v>
+        <v>2.651582759491257</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -1402,28 +1402,28 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>13.30366251056962</v>
+        <v>13.65883553855037</v>
       </c>
       <c r="G22">
-        <v>4317</v>
+        <v>4243</v>
       </c>
       <c r="H22">
-        <v>8.07403191514765</v>
+        <v>8.369779024329709</v>
       </c>
       <c r="I22">
-        <v>1.647709923664122</v>
+        <v>1.631923076923077</v>
       </c>
       <c r="J22">
-        <v>1.647709923664122</v>
+        <v>1.631923076923077</v>
       </c>
       <c r="K22">
-        <v>13.30366251056962</v>
+        <v>13.65883553855037</v>
       </c>
       <c r="L22">
-        <v>8.07403191514765</v>
+        <v>8.369779024329709</v>
       </c>
       <c r="M22">
-        <v>3.76626685674226</v>
+        <v>3.866816340963609</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1443,28 +1443,28 @@
         <v>76</v>
       </c>
       <c r="F23">
-        <v>13.39253973676282</v>
+        <v>13.57196208277016</v>
       </c>
       <c r="G23">
-        <v>4335</v>
+        <v>4236</v>
       </c>
       <c r="H23">
-        <v>8.094222401457575</v>
+        <v>8.33028834164363</v>
       </c>
       <c r="I23">
-        <v>1.654580152671756</v>
+        <v>1.629230769230769</v>
       </c>
       <c r="J23">
-        <v>125.7480916030534</v>
+        <v>123.8215384615385</v>
       </c>
       <c r="K23">
-        <v>1017.833019993974</v>
+        <v>1031.469118290532</v>
       </c>
       <c r="L23">
-        <v>615.1609025107757</v>
+        <v>633.1019139649159</v>
       </c>
       <c r="M23">
-        <v>2.122717548276907</v>
+        <v>2.15115599011907</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -1484,28 +1484,28 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>14.41687264993632</v>
+        <v>14.63407654354711</v>
       </c>
       <c r="G24">
-        <v>4672</v>
+        <v>4592</v>
       </c>
       <c r="H24">
-        <v>8.084804439818743</v>
+        <v>8.285844732844618</v>
       </c>
       <c r="I24">
-        <v>1.783206106870229</v>
+        <v>1.766153846153846</v>
       </c>
       <c r="J24">
-        <v>1.783206106870229</v>
+        <v>1.766153846153846</v>
       </c>
       <c r="K24">
-        <v>14.41687264993632</v>
+        <v>14.63407654354711</v>
       </c>
       <c r="L24">
-        <v>8.084804439818743</v>
+        <v>8.285844732844618</v>
       </c>
       <c r="M24">
-        <v>4.407237969085535</v>
+        <v>4.473637199362352</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -1522,25 +1522,25 @@
         <v>1183</v>
       </c>
       <c r="J25">
-        <v>1.425855471598278</v>
+        <v>1.423109760062423</v>
       </c>
       <c r="K25">
-        <v>9.770998203685073</v>
+        <v>10.13351681494935</v>
       </c>
       <c r="L25">
-        <v>6.852726940643225</v>
+        <v>7.120685346508236</v>
       </c>
       <c r="M25">
-        <v>51.46480950024928</v>
+        <v>53.17831914003776</v>
       </c>
       <c r="N25">
-        <v>2620</v>
+        <v>2600</v>
       </c>
       <c r="O25">
         <v>0.02</v>
       </c>
       <c r="P25">
-        <v>0.02088818228051634</v>
+        <v>0.02020916923218286</v>
       </c>
       <c r="Q25" t="s">
         <v>43</v>

</xml_diff>